<commit_message>
First standup and cleaned up the SCRUMs folder
</commit_message>
<xml_diff>
--- a/Algemeen/aanwezigheidslijst project game.xlsx
+++ b/Algemeen/aanwezigheidslijst project game.xlsx
@@ -159,6 +159,13 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
@@ -205,13 +212,6 @@
       <right style="thin"/>
       <top style="medium"/>
       <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -303,7 +303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="38">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -316,11 +316,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -332,11 +332,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -344,51 +344,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -540,7 +536,7 @@
   <dimension ref="A1:S19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -559,13 +555,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3"/>
       <c r="B3" s="0" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4"/>
       <c r="B4" s="5" t="s">
         <v>3</v>
@@ -578,7 +574,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="6"/>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="7"/>
       <c r="B5" s="5" t="s">
         <v>4</v>
@@ -587,7 +583,7 @@
       <c r="D5" s="5"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8"/>
       <c r="B6" s="9" t="s">
         <v>5</v>
@@ -598,13 +594,13 @@
       <c r="F6" s="9"/>
       <c r="G6" s="9"/>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10"/>
       <c r="B7" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="11"/>
       <c r="B8" s="12" t="s">
         <v>7</v>
@@ -660,112 +656,112 @@
       </c>
       <c r="B10" s="17"/>
       <c r="C10" s="18"/>
-      <c r="D10" s="19"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="21"/>
-      <c r="Q10" s="21"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="22"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19"/>
+      <c r="I10" s="19"/>
+      <c r="J10" s="19"/>
+      <c r="K10" s="19"/>
+      <c r="L10" s="19"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
+      <c r="O10" s="19"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="20"/>
+      <c r="S10" s="21"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="19"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="26"/>
-      <c r="G11" s="26"/>
-      <c r="H11" s="26"/>
-      <c r="I11" s="26"/>
-      <c r="J11" s="26"/>
-      <c r="K11" s="26"/>
-      <c r="L11" s="26"/>
-      <c r="M11" s="26"/>
-      <c r="N11" s="26"/>
-      <c r="O11" s="26"/>
-      <c r="P11" s="27"/>
-      <c r="Q11" s="27"/>
-      <c r="R11" s="27"/>
-      <c r="S11" s="28"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="25"/>
+      <c r="M11" s="25"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="25"/>
+      <c r="P11" s="26"/>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="26"/>
+      <c r="S11" s="27"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
-      <c r="J12" s="26"/>
-      <c r="K12" s="26"/>
-      <c r="L12" s="26"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="26"/>
-      <c r="O12" s="26"/>
-      <c r="P12" s="27"/>
-      <c r="Q12" s="27"/>
-      <c r="R12" s="27"/>
-      <c r="S12" s="28"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="25"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
+      <c r="I12" s="25"/>
+      <c r="J12" s="25"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="25"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="26"/>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="26"/>
+      <c r="S12" s="27"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="30"/>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
-      <c r="F13" s="32"/>
-      <c r="G13" s="32"/>
-      <c r="H13" s="32"/>
-      <c r="I13" s="32"/>
-      <c r="J13" s="32"/>
-      <c r="K13" s="32"/>
-      <c r="L13" s="32"/>
-      <c r="M13" s="32"/>
-      <c r="N13" s="32"/>
-      <c r="O13" s="32"/>
-      <c r="P13" s="33"/>
-      <c r="Q13" s="33"/>
-      <c r="R13" s="33"/>
-      <c r="S13" s="34"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
+      <c r="H13" s="31"/>
+      <c r="I13" s="31"/>
+      <c r="J13" s="31"/>
+      <c r="K13" s="31"/>
+      <c r="L13" s="31"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="31"/>
+      <c r="O13" s="31"/>
+      <c r="P13" s="32"/>
+      <c r="Q13" s="32"/>
+      <c r="R13" s="32"/>
+      <c r="S13" s="33"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="35"/>
-      <c r="B14" s="36"/>
-      <c r="C14" s="37"/>
-      <c r="D14" s="37"/>
-      <c r="E14" s="37"/>
-      <c r="F14" s="37"/>
-      <c r="G14" s="36"/>
-      <c r="H14" s="36"/>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="36"/>
-      <c r="N14" s="36"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="38"/>
-      <c r="Q14" s="38"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="38"/>
+      <c r="A14" s="34"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36"/>
+      <c r="E14" s="36"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="35"/>
+      <c r="H14" s="35"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="35"/>
+      <c r="L14" s="35"/>
+      <c r="M14" s="35"/>
+      <c r="N14" s="35"/>
+      <c r="O14" s="35"/>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="37"/>
+      <c r="S14" s="37"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>